<commit_message>
TP#20088: UK part 1
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1094,7 +1094,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2084,6 +2084,18 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="14" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2101,18 +2113,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="383">
@@ -2601,23 +2601,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2653,23 +2636,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2849,8 +2815,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:FB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,10 +2852,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:158" s="2" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="66" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3360,8 +3326,8 @@
       </c>
     </row>
     <row r="2" spans="1:158" s="2" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70"/>
-      <c r="B2" s="69"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="3"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11" t="s">
@@ -3831,7 +3797,7 @@
       <c r="A3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="67" t="s">
         <v>352</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -4155,7 +4121,7 @@
       <c r="A4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="64"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="25" t="s">
         <v>342</v>
       </c>
@@ -4471,7 +4437,7 @@
       <c r="A5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="25" t="s">
         <v>220</v>
       </c>
@@ -4811,7 +4777,7 @@
       <c r="A6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="25" t="s">
         <v>224</v>
       </c>
@@ -5109,7 +5075,7 @@
       <c r="A7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="25" t="s">
         <v>351</v>
       </c>
@@ -5407,7 +5373,7 @@
       <c r="A8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="25" t="s">
         <v>232</v>
       </c>
@@ -5755,7 +5721,7 @@
       <c r="A9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="25" t="s">
         <v>212</v>
       </c>
@@ -6061,7 +6027,7 @@
       <c r="A10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="64"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="25" t="s">
         <v>235</v>
       </c>
@@ -6407,7 +6373,7 @@
       <c r="A11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="64"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="25" t="s">
         <v>241</v>
       </c>
@@ -6749,7 +6715,7 @@
       <c r="A12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="64"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="25" t="s">
         <v>246</v>
       </c>
@@ -7093,7 +7059,7 @@
       <c r="A13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="64"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="25" t="s">
         <v>249</v>
       </c>
@@ -7397,7 +7363,7 @@
       <c r="A14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="64"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="25" t="s">
         <v>253</v>
       </c>
@@ -7747,7 +7713,7 @@
       <c r="A15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="64"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="25" t="s">
         <v>212</v>
       </c>
@@ -8069,7 +8035,7 @@
       <c r="A16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B16" s="64"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="25" t="s">
         <v>256</v>
       </c>
@@ -8371,7 +8337,7 @@
       <c r="A17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="25" t="s">
         <v>259</v>
       </c>
@@ -8687,7 +8653,7 @@
       <c r="A18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="25" t="s">
         <v>267</v>
       </c>
@@ -8983,7 +8949,7 @@
       <c r="A19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B19" s="64"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="25" t="s">
         <v>212</v>
       </c>
@@ -9291,7 +9257,7 @@
       <c r="A20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B20" s="64"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="25" t="s">
         <v>322</v>
       </c>
@@ -9659,7 +9625,7 @@
       <c r="A21" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="64"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="25" t="s">
         <v>275</v>
       </c>
@@ -9975,7 +9941,7 @@
       <c r="A22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="64"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="25" t="s">
         <v>338</v>
       </c>
@@ -10273,7 +10239,7 @@
       <c r="A23" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="64"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="25" t="s">
         <v>280</v>
       </c>
@@ -10593,7 +10559,7 @@
       <c r="A24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="64"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="25" t="s">
         <v>341</v>
       </c>
@@ -10947,7 +10913,7 @@
       <c r="A25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="64"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="25" t="s">
         <v>346</v>
       </c>
@@ -11323,7 +11289,7 @@
       <c r="A26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="64"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="25" t="s">
         <v>327</v>
       </c>
@@ -11643,7 +11609,7 @@
       <c r="A27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="64"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="25" t="s">
         <v>325</v>
       </c>
@@ -11963,7 +11929,7 @@
       <c r="A28" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="64"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="25" t="s">
         <v>220</v>
       </c>
@@ -12303,7 +12269,7 @@
       <c r="A29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="64"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="25" t="s">
         <v>295</v>
       </c>
@@ -12643,7 +12609,7 @@
       <c r="A30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="64"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="25" t="s">
         <v>253</v>
       </c>
@@ -12993,7 +12959,7 @@
       <c r="A31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="64"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="25" t="s">
         <v>235</v>
       </c>
@@ -13343,7 +13309,7 @@
       <c r="A32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="64"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="25" t="s">
         <v>302</v>
       </c>
@@ -13667,7 +13633,7 @@
       <c r="A33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="64"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="25" t="s">
         <v>324</v>
       </c>
@@ -13983,7 +13949,7 @@
       <c r="A34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="64"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="25" t="s">
         <v>343</v>
       </c>
@@ -14299,7 +14265,7 @@
       <c r="A35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="64"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="25" t="s">
         <v>326</v>
       </c>
@@ -14621,7 +14587,7 @@
       <c r="A36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="64"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="25" t="s">
         <v>309</v>
       </c>
@@ -14943,7 +14909,7 @@
       <c r="A37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="64"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="25" t="s">
         <v>337</v>
       </c>
@@ -15259,7 +15225,7 @@
       <c r="A38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="64"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="25" t="s">
         <v>312</v>
       </c>
@@ -15575,7 +15541,7 @@
       <c r="A39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="64"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="25" t="s">
         <v>316</v>
       </c>
@@ -15923,7 +15889,7 @@
       <c r="A40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="64"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="25" t="s">
         <v>173</v>
       </c>
@@ -16273,7 +16239,7 @@
       <c r="A41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B41" s="64"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="25" t="s">
         <v>319</v>
       </c>
@@ -16585,7 +16551,7 @@
       <c r="A42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B42" s="65"/>
+      <c r="B42" s="69"/>
       <c r="C42" s="30" t="s">
         <v>339</v>
       </c>
@@ -16903,7 +16869,7 @@
       <c r="A43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="70" t="s">
         <v>353</v>
       </c>
       <c r="C43" s="43" t="s">
@@ -17217,7 +17183,7 @@
       <c r="A44" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="67"/>
+      <c r="B44" s="71"/>
       <c r="C44" s="43" t="s">
         <v>323</v>
       </c>
@@ -17537,7 +17503,7 @@
       <c r="A45" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="67"/>
+      <c r="B45" s="71"/>
       <c r="C45" s="43" t="s">
         <v>340</v>
       </c>
@@ -17903,7 +17869,7 @@
       <c r="A46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="71"/>
       <c r="C46" s="43" t="s">
         <v>328</v>
       </c>
@@ -18225,7 +18191,7 @@
       <c r="A47" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="68"/>
+      <c r="B47" s="72"/>
       <c r="C47" s="43" t="s">
         <v>314</v>
       </c>

</xml_diff>

<commit_message>
TP#20444: Updated for failed UK tests
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
@@ -19,12 +19,12 @@
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="356">
   <si>
     <t>Description</t>
   </si>
@@ -1089,6 +1089,9 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>00133</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1216,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1247,6 +1250,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1898,7 +1907,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2095,6 +2104,42 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="51" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2815,8 +2860,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:FB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="DW1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="EJ1" sqref="EJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3797,7 +3842,7 @@
       <c r="A3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="79" t="s">
         <v>352</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -4121,7 +4166,7 @@
       <c r="A4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="68"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="25" t="s">
         <v>342</v>
       </c>
@@ -4242,8 +4287,8 @@
         <v>329</v>
       </c>
       <c r="AX4" s="35"/>
-      <c r="AY4" s="18">
-        <v>44030</v>
+      <c r="AY4" s="67" t="s">
+        <v>355</v>
       </c>
       <c r="AZ4" s="35" t="s">
         <v>168</v>
@@ -4437,7 +4482,7 @@
       <c r="A5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="68"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="25" t="s">
         <v>220</v>
       </c>
@@ -4773,309 +4818,309 @@
       <c r="FA5" s="26"/>
       <c r="FB5" s="28"/>
     </row>
-    <row r="6" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="b">
+    <row r="6" spans="1:158" s="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="80"/>
+      <c r="C6" s="69" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35" t="s">
+      <c r="F6" s="71"/>
+      <c r="G6" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="J6" s="35">
-        <v>30</v>
-      </c>
-      <c r="K6" s="35" t="s">
+      <c r="J6" s="71">
+        <v>10</v>
+      </c>
+      <c r="K6" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="71">
         <v>605517846</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="Q6" s="35" t="s">
+      <c r="Q6" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="R6" s="38" t="s">
+      <c r="R6" s="74" t="s">
         <v>344</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35" t="s">
+      <c r="T6" s="71"/>
+      <c r="U6" s="71" t="s">
         <v>345</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="V6" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="W6" s="35" t="s">
+      <c r="W6" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="X6" s="35" t="s">
+      <c r="X6" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="Y6" s="35" t="s">
+      <c r="Y6" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="Z6" s="35" t="s">
+      <c r="Z6" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="AA6" s="35" t="s">
+      <c r="AA6" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="AB6" s="35" t="s">
+      <c r="AB6" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="AC6" s="35">
+      <c r="AC6" s="71">
         <v>15520</v>
       </c>
-      <c r="AD6" s="35" t="s">
+      <c r="AD6" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="AE6" s="35" t="s">
+      <c r="AE6" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="AF6" s="35" t="s">
+      <c r="AF6" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="AG6" s="26" t="s">
+      <c r="AG6" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="AH6" s="59" t="s">
+      <c r="AH6" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="35"/>
-      <c r="AO6" s="35"/>
-      <c r="AP6" s="35"/>
-      <c r="AQ6" s="35"/>
-      <c r="AR6" s="35"/>
-      <c r="AS6" s="35"/>
-      <c r="AT6" s="35"/>
-      <c r="AU6" s="35"/>
-      <c r="AV6" s="35"/>
-      <c r="AW6" s="35"/>
-      <c r="AX6" s="35"/>
-      <c r="AY6" s="18"/>
-      <c r="AZ6" s="35"/>
-      <c r="BA6" s="35"/>
-      <c r="BB6" s="17"/>
-      <c r="BC6" s="17"/>
-      <c r="BD6" s="17"/>
-      <c r="BE6" s="35"/>
-      <c r="BF6" s="35"/>
-      <c r="BG6" s="35"/>
-      <c r="BH6" s="35"/>
-      <c r="BI6" s="35"/>
-      <c r="BJ6" s="35"/>
-      <c r="BK6" s="35"/>
-      <c r="BL6" s="35"/>
-      <c r="BM6" s="35"/>
-      <c r="BN6" s="35"/>
-      <c r="BO6" s="35"/>
-      <c r="BP6" s="35"/>
-      <c r="BQ6" s="35"/>
-      <c r="BR6" s="35"/>
-      <c r="BS6" s="35"/>
-      <c r="BT6" s="35"/>
-      <c r="BU6" s="35"/>
-      <c r="BV6" s="35"/>
-      <c r="BW6" s="35"/>
-      <c r="BX6" s="35"/>
-      <c r="BY6" s="35"/>
-      <c r="BZ6" s="35"/>
-      <c r="CA6" s="35"/>
-      <c r="CB6" s="35"/>
-      <c r="CC6" s="35"/>
-      <c r="CD6" s="35"/>
-      <c r="CE6" s="35"/>
-      <c r="CF6" s="35"/>
-      <c r="CG6" s="35"/>
-      <c r="CH6" s="35"/>
-      <c r="CI6" s="35"/>
-      <c r="CJ6" s="54" t="s">
+      <c r="AI6" s="71"/>
+      <c r="AJ6" s="71"/>
+      <c r="AK6" s="71"/>
+      <c r="AL6" s="71"/>
+      <c r="AM6" s="71"/>
+      <c r="AN6" s="71"/>
+      <c r="AO6" s="71"/>
+      <c r="AP6" s="71"/>
+      <c r="AQ6" s="71"/>
+      <c r="AR6" s="71"/>
+      <c r="AS6" s="71"/>
+      <c r="AT6" s="71"/>
+      <c r="AU6" s="71"/>
+      <c r="AV6" s="71"/>
+      <c r="AW6" s="71"/>
+      <c r="AX6" s="71"/>
+      <c r="AY6" s="76"/>
+      <c r="AZ6" s="71"/>
+      <c r="BA6" s="71"/>
+      <c r="BB6" s="73"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="73"/>
+      <c r="BE6" s="71"/>
+      <c r="BF6" s="71"/>
+      <c r="BG6" s="71"/>
+      <c r="BH6" s="71"/>
+      <c r="BI6" s="71"/>
+      <c r="BJ6" s="71"/>
+      <c r="BK6" s="71"/>
+      <c r="BL6" s="71"/>
+      <c r="BM6" s="71"/>
+      <c r="BN6" s="71"/>
+      <c r="BO6" s="71"/>
+      <c r="BP6" s="71"/>
+      <c r="BQ6" s="71"/>
+      <c r="BR6" s="71"/>
+      <c r="BS6" s="71"/>
+      <c r="BT6" s="71"/>
+      <c r="BU6" s="71"/>
+      <c r="BV6" s="71"/>
+      <c r="BW6" s="71"/>
+      <c r="BX6" s="71"/>
+      <c r="BY6" s="71"/>
+      <c r="BZ6" s="71"/>
+      <c r="CA6" s="71"/>
+      <c r="CB6" s="71"/>
+      <c r="CC6" s="71"/>
+      <c r="CD6" s="71"/>
+      <c r="CE6" s="71"/>
+      <c r="CF6" s="71"/>
+      <c r="CG6" s="71"/>
+      <c r="CH6" s="71"/>
+      <c r="CI6" s="71"/>
+      <c r="CJ6" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="CK6" s="54" t="s">
+      <c r="CK6" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="CL6" s="35" t="s">
+      <c r="CL6" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="CM6" s="59" t="s">
+      <c r="CM6" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="CN6" s="26" t="s">
+      <c r="CN6" s="70" t="s">
         <v>151</v>
       </c>
-      <c r="CO6" s="26" t="s">
+      <c r="CO6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="CP6" s="26">
+      <c r="CP6" s="70">
         <v>1000</v>
       </c>
-      <c r="CQ6" s="26" t="s">
+      <c r="CQ6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="CR6" s="26">
+      <c r="CR6" s="70">
         <v>100</v>
       </c>
-      <c r="CS6" s="26" t="s">
+      <c r="CS6" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="CT6" s="26" t="s">
+      <c r="CT6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="CU6" s="26">
+      <c r="CU6" s="70">
         <v>100</v>
       </c>
-      <c r="CV6" s="26" t="s">
+      <c r="CV6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="CW6" s="26">
+      <c r="CW6" s="70">
         <v>25</v>
       </c>
-      <c r="CX6" s="26" t="s">
+      <c r="CX6" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="CY6" s="26" t="s">
+      <c r="CY6" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="CZ6" s="26">
+      <c r="CZ6" s="70">
         <v>123456789</v>
       </c>
-      <c r="DA6" s="26"/>
-      <c r="DB6" s="26"/>
-      <c r="DC6" s="26">
+      <c r="DA6" s="70"/>
+      <c r="DB6" s="70"/>
+      <c r="DC6" s="70">
         <v>1</v>
       </c>
-      <c r="DD6" s="26" t="s">
+      <c r="DD6" s="70" t="s">
         <v>229</v>
       </c>
-      <c r="DE6" s="26" t="s">
+      <c r="DE6" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="DF6" s="26"/>
-      <c r="DG6" s="26" t="s">
+      <c r="DF6" s="70"/>
+      <c r="DG6" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="DH6" s="35">
-        <v>30</v>
-      </c>
-      <c r="DI6" s="26">
+      <c r="DH6" s="71">
+        <v>10</v>
+      </c>
+      <c r="DI6" s="70">
         <v>1</v>
       </c>
-      <c r="DJ6" s="26" t="s">
+      <c r="DJ6" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="DK6" s="26" t="s">
+      <c r="DK6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="DL6" s="26">
+      <c r="DL6" s="70">
         <v>100</v>
       </c>
-      <c r="DM6" s="26" t="s">
+      <c r="DM6" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="DN6" s="26">
+      <c r="DN6" s="70">
         <v>10000</v>
       </c>
-      <c r="DO6" s="26" t="s">
+      <c r="DO6" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="DP6" s="35" t="s">
+      <c r="DP6" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="DQ6" s="35" t="s">
+      <c r="DQ6" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="DR6" s="26">
+      <c r="DR6" s="70">
         <v>1</v>
       </c>
-      <c r="DS6" s="35" t="s">
+      <c r="DS6" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="DT6" s="35">
+      <c r="DT6" s="71">
         <v>100</v>
       </c>
-      <c r="DU6" s="35" t="s">
+      <c r="DU6" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="DV6" s="35">
-        <v>30</v>
-      </c>
-      <c r="DW6" s="35"/>
-      <c r="DX6" s="35"/>
-      <c r="DY6" s="35"/>
-      <c r="DZ6" s="35"/>
-      <c r="EA6" s="35" t="s">
+      <c r="DV6" s="71">
+        <v>10</v>
+      </c>
+      <c r="DW6" s="71"/>
+      <c r="DX6" s="71"/>
+      <c r="DY6" s="71"/>
+      <c r="DZ6" s="71"/>
+      <c r="EA6" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="EB6" s="35" t="s">
+      <c r="EB6" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="EC6" s="35"/>
-      <c r="ED6" s="35"/>
-      <c r="EE6" s="35"/>
-      <c r="EF6" s="35"/>
-      <c r="EG6" s="35"/>
-      <c r="EH6" s="35"/>
-      <c r="EI6" s="35"/>
-      <c r="EJ6" s="35"/>
-      <c r="EK6" s="35"/>
-      <c r="EL6" s="35"/>
-      <c r="EM6" s="26"/>
-      <c r="EN6" s="26"/>
-      <c r="EO6" s="26"/>
-      <c r="EP6" s="26"/>
-      <c r="EQ6" s="26"/>
-      <c r="ER6" s="26"/>
-      <c r="ES6" s="26"/>
-      <c r="ET6" s="26"/>
-      <c r="EU6" s="26"/>
-      <c r="EV6" s="26"/>
-      <c r="EW6" s="26"/>
-      <c r="EX6" s="26"/>
-      <c r="EY6" s="26"/>
-      <c r="EZ6" s="26"/>
-      <c r="FA6" s="26"/>
-      <c r="FB6" s="28"/>
+      <c r="EC6" s="71"/>
+      <c r="ED6" s="71"/>
+      <c r="EE6" s="71"/>
+      <c r="EF6" s="71"/>
+      <c r="EG6" s="71"/>
+      <c r="EH6" s="71"/>
+      <c r="EI6" s="71"/>
+      <c r="EJ6" s="71"/>
+      <c r="EK6" s="71"/>
+      <c r="EL6" s="71"/>
+      <c r="EM6" s="70"/>
+      <c r="EN6" s="70"/>
+      <c r="EO6" s="70"/>
+      <c r="EP6" s="70"/>
+      <c r="EQ6" s="70"/>
+      <c r="ER6" s="70"/>
+      <c r="ES6" s="70"/>
+      <c r="ET6" s="70"/>
+      <c r="EU6" s="70"/>
+      <c r="EV6" s="70"/>
+      <c r="EW6" s="70"/>
+      <c r="EX6" s="70"/>
+      <c r="EY6" s="70"/>
+      <c r="EZ6" s="70"/>
+      <c r="FA6" s="70"/>
+      <c r="FB6" s="78"/>
     </row>
     <row r="7" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="68"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="25" t="s">
         <v>351</v>
       </c>
@@ -5373,7 +5418,7 @@
       <c r="A8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="25" t="s">
         <v>232</v>
       </c>
@@ -5721,7 +5766,7 @@
       <c r="A9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="68"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="25" t="s">
         <v>212</v>
       </c>
@@ -6027,7 +6072,7 @@
       <c r="A10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="68"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="25" t="s">
         <v>235</v>
       </c>
@@ -6373,7 +6418,7 @@
       <c r="A11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="68"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="25" t="s">
         <v>241</v>
       </c>
@@ -6715,7 +6760,7 @@
       <c r="A12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="68"/>
+      <c r="B12" s="80"/>
       <c r="C12" s="25" t="s">
         <v>246</v>
       </c>
@@ -7059,7 +7104,7 @@
       <c r="A13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="68"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="25" t="s">
         <v>249</v>
       </c>
@@ -7359,361 +7404,361 @@
       <c r="FA13" s="26"/>
       <c r="FB13" s="28"/>
     </row>
-    <row r="14" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="b">
+    <row r="14" spans="1:158" s="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="80"/>
+      <c r="C14" s="69" t="s">
         <v>253</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="71" t="s">
         <v>250</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35" t="s">
+      <c r="F14" s="71"/>
+      <c r="G14" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="35">
+      <c r="J14" s="71">
+        <v>150</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="L14" s="71">
+        <v>605517846</v>
+      </c>
+      <c r="M14" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="N14" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="O14" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="P14" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q14" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="R14" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="S14" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="T14" s="71"/>
+      <c r="U14" s="71" t="s">
+        <v>345</v>
+      </c>
+      <c r="V14" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="W14" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="X14" s="71" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y14" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z14" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA14" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB14" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC14" s="71">
+        <v>30339</v>
+      </c>
+      <c r="AD14" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE14" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF14" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="AG14" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH14" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI14" s="71" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ14" s="71"/>
+      <c r="AK14" s="71"/>
+      <c r="AL14" s="71"/>
+      <c r="AM14" s="71"/>
+      <c r="AN14" s="71"/>
+      <c r="AO14" s="71"/>
+      <c r="AP14" s="71"/>
+      <c r="AQ14" s="71"/>
+      <c r="AR14" s="71"/>
+      <c r="AS14" s="71"/>
+      <c r="AT14" s="71"/>
+      <c r="AU14" s="71"/>
+      <c r="AV14" s="71"/>
+      <c r="AW14" s="71"/>
+      <c r="AX14" s="71"/>
+      <c r="AY14" s="76"/>
+      <c r="AZ14" s="71"/>
+      <c r="BA14" s="71"/>
+      <c r="BB14" s="73">
+        <v>1</v>
+      </c>
+      <c r="BC14" s="73" t="s">
+        <v>349</v>
+      </c>
+      <c r="BD14" s="73" t="s">
+        <v>350</v>
+      </c>
+      <c r="BE14" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="BF14" s="71">
+        <v>222326460</v>
+      </c>
+      <c r="BG14" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="BH14" s="71">
+        <v>1234567890</v>
+      </c>
+      <c r="BI14" s="71">
+        <v>12345</v>
+      </c>
+      <c r="BJ14" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="BK14" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="BL14" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM14" s="71">
+        <v>8975898616</v>
+      </c>
+      <c r="BN14" s="71">
+        <v>3293</v>
+      </c>
+      <c r="BO14" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="BP14" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="BQ14" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="BR14" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="BS14" s="71">
+        <v>30339</v>
+      </c>
+      <c r="BT14" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="BU14" s="71"/>
+      <c r="BV14" s="71"/>
+      <c r="BW14" s="71"/>
+      <c r="BX14" s="71"/>
+      <c r="BY14" s="71"/>
+      <c r="BZ14" s="71"/>
+      <c r="CA14" s="71"/>
+      <c r="CB14" s="71"/>
+      <c r="CC14" s="71"/>
+      <c r="CD14" s="71"/>
+      <c r="CE14" s="71"/>
+      <c r="CF14" s="71"/>
+      <c r="CG14" s="71"/>
+      <c r="CH14" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="CI14" s="71">
+        <v>123456789</v>
+      </c>
+      <c r="CJ14" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="CK14" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="CL14" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="CM14" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN14" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="CO14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="CP14" s="70">
+        <v>2000</v>
+      </c>
+      <c r="CQ14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="CR14" s="70">
+        <v>50</v>
+      </c>
+      <c r="CS14" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="CT14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="CU14" s="70">
+        <v>100</v>
+      </c>
+      <c r="CV14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="CW14" s="70">
+        <v>25</v>
+      </c>
+      <c r="CX14" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="CY14" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="CZ14" s="70">
+        <v>123456789</v>
+      </c>
+      <c r="DA14" s="70"/>
+      <c r="DB14" s="70"/>
+      <c r="DC14" s="70">
+        <v>1</v>
+      </c>
+      <c r="DD14" s="70" t="s">
+        <v>156</v>
+      </c>
+      <c r="DE14" s="70" t="s">
+        <v>203</v>
+      </c>
+      <c r="DF14" s="70"/>
+      <c r="DG14" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="DH14" s="71">
         <v>10</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="DI14" s="70">
+        <v>1</v>
+      </c>
+      <c r="DJ14" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="DK14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="DL14" s="70">
+        <v>100</v>
+      </c>
+      <c r="DM14" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="DN14" s="70">
+        <v>2000</v>
+      </c>
+      <c r="DO14" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="DP14" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="DQ14" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="DR14" s="70">
+        <v>1</v>
+      </c>
+      <c r="DS14" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="DT14" s="71">
+        <v>800</v>
+      </c>
+      <c r="DU14" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="L14" s="35">
-        <v>605517846</v>
-      </c>
-      <c r="M14" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="N14" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="O14" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="P14" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q14" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="R14" s="38" t="s">
-        <v>344</v>
-      </c>
-      <c r="S14" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35" t="s">
-        <v>345</v>
-      </c>
-      <c r="V14" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="W14" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="X14" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y14" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z14" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA14" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB14" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC14" s="35">
-        <v>30339</v>
-      </c>
-      <c r="AD14" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE14" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF14" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="AG14" s="26" t="s">
+      <c r="DV14" s="71">
+        <v>10</v>
+      </c>
+      <c r="DW14" s="71">
+        <v>120</v>
+      </c>
+      <c r="DX14" s="71">
+        <v>60</v>
+      </c>
+      <c r="DY14" s="71">
+        <v>60</v>
+      </c>
+      <c r="DZ14" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="EA14" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="EB14" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="AH14" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI14" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="AJ14" s="35"/>
-      <c r="AK14" s="35"/>
-      <c r="AL14" s="35"/>
-      <c r="AM14" s="35"/>
-      <c r="AN14" s="35"/>
-      <c r="AO14" s="35"/>
-      <c r="AP14" s="35"/>
-      <c r="AQ14" s="35"/>
-      <c r="AR14" s="35"/>
-      <c r="AS14" s="35"/>
-      <c r="AT14" s="35"/>
-      <c r="AU14" s="35"/>
-      <c r="AV14" s="35"/>
-      <c r="AW14" s="35"/>
-      <c r="AX14" s="35"/>
-      <c r="AY14" s="18"/>
-      <c r="AZ14" s="35"/>
-      <c r="BA14" s="35"/>
-      <c r="BB14" s="17">
-        <v>1</v>
-      </c>
-      <c r="BC14" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="BD14" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="BE14" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="BF14" s="35">
-        <v>222326460</v>
-      </c>
-      <c r="BG14" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="BH14" s="35">
-        <v>1234567890</v>
-      </c>
-      <c r="BI14" s="35">
-        <v>12345</v>
-      </c>
-      <c r="BJ14" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="BK14" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="BL14" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="BM14" s="35">
-        <v>8975898616</v>
-      </c>
-      <c r="BN14" s="35">
-        <v>3293</v>
-      </c>
-      <c r="BO14" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="BP14" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="BQ14" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="BR14" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="BS14" s="35">
-        <v>30339</v>
-      </c>
-      <c r="BT14" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="BU14" s="35"/>
-      <c r="BV14" s="35"/>
-      <c r="BW14" s="35"/>
-      <c r="BX14" s="35"/>
-      <c r="BY14" s="35"/>
-      <c r="BZ14" s="35"/>
-      <c r="CA14" s="35"/>
-      <c r="CB14" s="35"/>
-      <c r="CC14" s="35"/>
-      <c r="CD14" s="35"/>
-      <c r="CE14" s="35"/>
-      <c r="CF14" s="35"/>
-      <c r="CG14" s="35"/>
-      <c r="CH14" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="CI14" s="35">
-        <v>123456789</v>
-      </c>
-      <c r="CJ14" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="CK14" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="CL14" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="CM14" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="CN14" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="CO14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="CP14" s="26">
-        <v>2000</v>
-      </c>
-      <c r="CQ14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="CR14" s="26">
-        <v>50</v>
-      </c>
-      <c r="CS14" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="CT14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="CU14" s="26">
-        <v>100</v>
-      </c>
-      <c r="CV14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="CW14" s="26">
-        <v>25</v>
-      </c>
-      <c r="CX14" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="CY14" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="CZ14" s="26">
-        <v>123456789</v>
-      </c>
-      <c r="DA14" s="26"/>
-      <c r="DB14" s="26"/>
-      <c r="DC14" s="26">
-        <v>1</v>
-      </c>
-      <c r="DD14" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="DE14" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="DF14" s="26"/>
-      <c r="DG14" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="DH14" s="35">
-        <v>10</v>
-      </c>
-      <c r="DI14" s="26">
-        <v>1</v>
-      </c>
-      <c r="DJ14" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="DK14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="DL14" s="26">
-        <v>100</v>
-      </c>
-      <c r="DM14" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="DN14" s="26">
-        <v>2000</v>
-      </c>
-      <c r="DO14" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="DP14" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="DQ14" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="DR14" s="26">
-        <v>1</v>
-      </c>
-      <c r="DS14" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="DT14" s="35">
-        <v>800</v>
-      </c>
-      <c r="DU14" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="DV14" s="35">
-        <v>10</v>
-      </c>
-      <c r="DW14" s="35">
-        <v>20</v>
-      </c>
-      <c r="DX14" s="35">
-        <v>20</v>
-      </c>
-      <c r="DY14" s="35">
-        <v>20</v>
-      </c>
-      <c r="DZ14" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="EA14" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="EB14" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="EC14" s="35"/>
-      <c r="ED14" s="35"/>
-      <c r="EE14" s="35"/>
-      <c r="EF14" s="35"/>
-      <c r="EG14" s="35"/>
-      <c r="EH14" s="35"/>
-      <c r="EI14" s="35"/>
-      <c r="EJ14" s="35"/>
-      <c r="EK14" s="35"/>
-      <c r="EL14" s="35"/>
-      <c r="EM14" s="26"/>
-      <c r="EN14" s="26"/>
-      <c r="EO14" s="26"/>
-      <c r="EP14" s="26"/>
-      <c r="EQ14" s="26"/>
-      <c r="ER14" s="26"/>
-      <c r="ES14" s="26"/>
-      <c r="ET14" s="26"/>
-      <c r="EU14" s="26"/>
-      <c r="EV14" s="26"/>
-      <c r="EW14" s="26"/>
-      <c r="EX14" s="26"/>
-      <c r="EY14" s="26"/>
-      <c r="EZ14" s="26"/>
-      <c r="FA14" s="26"/>
-      <c r="FB14" s="28"/>
+      <c r="EC14" s="71"/>
+      <c r="ED14" s="71"/>
+      <c r="EE14" s="71"/>
+      <c r="EF14" s="71"/>
+      <c r="EG14" s="71"/>
+      <c r="EH14" s="71"/>
+      <c r="EI14" s="71"/>
+      <c r="EJ14" s="71"/>
+      <c r="EK14" s="71"/>
+      <c r="EL14" s="71"/>
+      <c r="EM14" s="70"/>
+      <c r="EN14" s="70"/>
+      <c r="EO14" s="70"/>
+      <c r="EP14" s="70"/>
+      <c r="EQ14" s="70"/>
+      <c r="ER14" s="70"/>
+      <c r="ES14" s="70"/>
+      <c r="ET14" s="70"/>
+      <c r="EU14" s="70"/>
+      <c r="EV14" s="70"/>
+      <c r="EW14" s="70"/>
+      <c r="EX14" s="70"/>
+      <c r="EY14" s="70"/>
+      <c r="EZ14" s="70"/>
+      <c r="FA14" s="70"/>
+      <c r="FB14" s="78"/>
     </row>
     <row r="15" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="68"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="25" t="s">
         <v>212</v>
       </c>
@@ -8035,7 +8080,7 @@
       <c r="A16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B16" s="68"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="25" t="s">
         <v>256</v>
       </c>
@@ -8337,7 +8382,7 @@
       <c r="A17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="68"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="25" t="s">
         <v>259</v>
       </c>
@@ -8649,307 +8694,307 @@
       <c r="FA17" s="26"/>
       <c r="FB17" s="28"/>
     </row>
-    <row r="18" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="b">
+    <row r="18" spans="1:158" s="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="69" t="s">
         <v>267</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35" t="s">
+      <c r="F18" s="71"/>
+      <c r="G18" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="J18" s="35">
-        <v>11</v>
-      </c>
-      <c r="K18" s="35" t="s">
+      <c r="J18" s="71">
+        <v>1</v>
+      </c>
+      <c r="K18" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="L18" s="35">
+      <c r="L18" s="71">
         <v>605517846</v>
       </c>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="O18" s="35" t="s">
+      <c r="O18" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="35" t="s">
+      <c r="P18" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="Q18" s="35" t="s">
+      <c r="Q18" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="R18" s="38" t="s">
+      <c r="R18" s="74" t="s">
         <v>344</v>
       </c>
-      <c r="S18" s="35" t="s">
+      <c r="S18" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35" t="s">
+      <c r="T18" s="71"/>
+      <c r="U18" s="71" t="s">
         <v>345</v>
       </c>
-      <c r="V18" s="35" t="s">
+      <c r="V18" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="W18" s="35" t="s">
+      <c r="W18" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="X18" s="35" t="s">
+      <c r="X18" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="Y18" s="35">
+      <c r="Y18" s="71">
         <v>61293286200</v>
       </c>
-      <c r="Z18" s="35" t="s">
+      <c r="Z18" s="71" t="s">
         <v>269</v>
       </c>
-      <c r="AA18" s="35" t="s">
+      <c r="AA18" s="71" t="s">
         <v>270</v>
       </c>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35">
+      <c r="AB18" s="71"/>
+      <c r="AC18" s="71">
         <v>2028</v>
       </c>
-      <c r="AD18" s="35" t="s">
+      <c r="AD18" s="71" t="s">
         <v>271</v>
       </c>
-      <c r="AE18" s="35" t="s">
+      <c r="AE18" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="AF18" s="35">
+      <c r="AF18" s="71">
         <v>150067600</v>
       </c>
-      <c r="AG18" s="26" t="s">
+      <c r="AG18" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="AH18" s="59" t="s">
+      <c r="AH18" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="AI18" s="35"/>
-      <c r="AJ18" s="35"/>
-      <c r="AK18" s="35"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="35"/>
-      <c r="AN18" s="35"/>
-      <c r="AO18" s="35"/>
-      <c r="AP18" s="35"/>
-      <c r="AQ18" s="35"/>
-      <c r="AR18" s="35"/>
-      <c r="AS18" s="35"/>
-      <c r="AT18" s="35"/>
-      <c r="AU18" s="35"/>
-      <c r="AV18" s="35"/>
-      <c r="AW18" s="35"/>
-      <c r="AX18" s="35"/>
-      <c r="AY18" s="18"/>
-      <c r="AZ18" s="35"/>
-      <c r="BA18" s="35"/>
-      <c r="BB18" s="17"/>
-      <c r="BC18" s="17"/>
-      <c r="BD18" s="17"/>
-      <c r="BE18" s="35"/>
-      <c r="BF18" s="35"/>
-      <c r="BG18" s="35"/>
-      <c r="BH18" s="35"/>
-      <c r="BI18" s="35"/>
-      <c r="BJ18" s="35"/>
-      <c r="BK18" s="35"/>
-      <c r="BL18" s="35"/>
-      <c r="BM18" s="35"/>
-      <c r="BN18" s="35"/>
-      <c r="BO18" s="35"/>
-      <c r="BP18" s="35"/>
-      <c r="BQ18" s="35"/>
-      <c r="BR18" s="35"/>
-      <c r="BS18" s="35"/>
-      <c r="BT18" s="35"/>
-      <c r="BU18" s="35"/>
-      <c r="BV18" s="35"/>
-      <c r="BW18" s="35"/>
-      <c r="BX18" s="35"/>
-      <c r="BY18" s="35"/>
-      <c r="BZ18" s="35"/>
-      <c r="CA18" s="35"/>
-      <c r="CB18" s="35"/>
-      <c r="CC18" s="35"/>
-      <c r="CD18" s="35"/>
-      <c r="CE18" s="35"/>
-      <c r="CF18" s="35"/>
-      <c r="CG18" s="35"/>
-      <c r="CH18" s="35"/>
-      <c r="CI18" s="35"/>
-      <c r="CJ18" s="54" t="s">
+      <c r="AI18" s="71"/>
+      <c r="AJ18" s="71"/>
+      <c r="AK18" s="71"/>
+      <c r="AL18" s="71"/>
+      <c r="AM18" s="71"/>
+      <c r="AN18" s="71"/>
+      <c r="AO18" s="71"/>
+      <c r="AP18" s="71"/>
+      <c r="AQ18" s="71"/>
+      <c r="AR18" s="71"/>
+      <c r="AS18" s="71"/>
+      <c r="AT18" s="71"/>
+      <c r="AU18" s="71"/>
+      <c r="AV18" s="71"/>
+      <c r="AW18" s="71"/>
+      <c r="AX18" s="71"/>
+      <c r="AY18" s="76"/>
+      <c r="AZ18" s="71"/>
+      <c r="BA18" s="71"/>
+      <c r="BB18" s="73"/>
+      <c r="BC18" s="73"/>
+      <c r="BD18" s="73"/>
+      <c r="BE18" s="71"/>
+      <c r="BF18" s="71"/>
+      <c r="BG18" s="71"/>
+      <c r="BH18" s="71"/>
+      <c r="BI18" s="71"/>
+      <c r="BJ18" s="71"/>
+      <c r="BK18" s="71"/>
+      <c r="BL18" s="71"/>
+      <c r="BM18" s="71"/>
+      <c r="BN18" s="71"/>
+      <c r="BO18" s="71"/>
+      <c r="BP18" s="71"/>
+      <c r="BQ18" s="71"/>
+      <c r="BR18" s="71"/>
+      <c r="BS18" s="71"/>
+      <c r="BT18" s="71"/>
+      <c r="BU18" s="71"/>
+      <c r="BV18" s="71"/>
+      <c r="BW18" s="71"/>
+      <c r="BX18" s="71"/>
+      <c r="BY18" s="71"/>
+      <c r="BZ18" s="71"/>
+      <c r="CA18" s="71"/>
+      <c r="CB18" s="71"/>
+      <c r="CC18" s="71"/>
+      <c r="CD18" s="71"/>
+      <c r="CE18" s="71"/>
+      <c r="CF18" s="71"/>
+      <c r="CG18" s="71"/>
+      <c r="CH18" s="71"/>
+      <c r="CI18" s="71"/>
+      <c r="CJ18" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="CK18" s="54">
+      <c r="CK18" s="77">
         <v>214877600</v>
       </c>
-      <c r="CL18" s="35" t="s">
+      <c r="CL18" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="CM18" s="59" t="s">
+      <c r="CM18" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="CN18" s="26" t="s">
+      <c r="CN18" s="70" t="s">
         <v>151</v>
       </c>
-      <c r="CO18" s="26" t="s">
+      <c r="CO18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="CP18" s="26">
+      <c r="CP18" s="70">
         <v>200</v>
       </c>
-      <c r="CQ18" s="26" t="s">
+      <c r="CQ18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="CR18" s="26">
+      <c r="CR18" s="70">
         <v>10</v>
       </c>
-      <c r="CS18" s="26" t="s">
+      <c r="CS18" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="CT18" s="26" t="s">
+      <c r="CT18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="CU18" s="26">
+      <c r="CU18" s="70">
         <v>100</v>
       </c>
-      <c r="CV18" s="26" t="s">
+      <c r="CV18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="CW18" s="26">
+      <c r="CW18" s="70">
         <v>25</v>
       </c>
-      <c r="CX18" s="26" t="s">
+      <c r="CX18" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="CY18" s="26" t="s">
+      <c r="CY18" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="CZ18" s="26">
+      <c r="CZ18" s="70">
         <v>123456789</v>
       </c>
-      <c r="DA18" s="26"/>
-      <c r="DB18" s="26"/>
-      <c r="DC18" s="26">
+      <c r="DA18" s="70"/>
+      <c r="DB18" s="70"/>
+      <c r="DC18" s="70">
         <v>1</v>
       </c>
-      <c r="DD18" s="26" t="s">
+      <c r="DD18" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="DE18" s="26" t="s">
+      <c r="DE18" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="DF18" s="26"/>
-      <c r="DG18" s="26" t="s">
+      <c r="DF18" s="70"/>
+      <c r="DG18" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="DH18" s="35">
-        <v>11</v>
-      </c>
-      <c r="DI18" s="26">
+      <c r="DH18" s="71">
         <v>1</v>
       </c>
-      <c r="DJ18" s="26" t="s">
+      <c r="DI18" s="70">
+        <v>1</v>
+      </c>
+      <c r="DJ18" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="DK18" s="26" t="s">
+      <c r="DK18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="DL18" s="26">
+      <c r="DL18" s="70">
         <v>100</v>
       </c>
-      <c r="DM18" s="26" t="s">
+      <c r="DM18" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="DN18" s="26">
+      <c r="DN18" s="70">
         <v>200</v>
       </c>
-      <c r="DO18" s="26" t="s">
+      <c r="DO18" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="DP18" s="35" t="s">
+      <c r="DP18" s="71" t="s">
         <v>160</v>
       </c>
-      <c r="DQ18" s="35" t="s">
+      <c r="DQ18" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="DR18" s="26">
+      <c r="DR18" s="70">
         <v>1</v>
       </c>
-      <c r="DS18" s="35" t="s">
+      <c r="DS18" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="DT18" s="35">
+      <c r="DT18" s="71">
         <v>66</v>
       </c>
-      <c r="DU18" s="35" t="s">
+      <c r="DU18" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="DV18" s="35">
-        <v>11</v>
-      </c>
-      <c r="DW18" s="35"/>
-      <c r="DX18" s="35"/>
-      <c r="DY18" s="35"/>
-      <c r="DZ18" s="35"/>
-      <c r="EA18" s="35" t="s">
+      <c r="DV18" s="71">
+        <v>1</v>
+      </c>
+      <c r="DW18" s="71"/>
+      <c r="DX18" s="71"/>
+      <c r="DY18" s="71"/>
+      <c r="DZ18" s="71"/>
+      <c r="EA18" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="EB18" s="35" t="s">
+      <c r="EB18" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="EC18" s="35"/>
-      <c r="ED18" s="35"/>
-      <c r="EE18" s="35"/>
-      <c r="EF18" s="35"/>
-      <c r="EG18" s="35"/>
-      <c r="EH18" s="35"/>
-      <c r="EI18" s="35"/>
-      <c r="EJ18" s="35"/>
-      <c r="EK18" s="35"/>
-      <c r="EL18" s="35"/>
-      <c r="EM18" s="26"/>
-      <c r="EN18" s="26"/>
-      <c r="EO18" s="26"/>
-      <c r="EP18" s="26"/>
-      <c r="EQ18" s="26"/>
-      <c r="ER18" s="26"/>
-      <c r="ES18" s="26"/>
-      <c r="ET18" s="26"/>
-      <c r="EU18" s="26"/>
-      <c r="EV18" s="26"/>
-      <c r="EW18" s="26"/>
-      <c r="EX18" s="26"/>
-      <c r="EY18" s="26"/>
-      <c r="EZ18" s="26"/>
-      <c r="FA18" s="26"/>
-      <c r="FB18" s="28"/>
+      <c r="EC18" s="71"/>
+      <c r="ED18" s="71"/>
+      <c r="EE18" s="71"/>
+      <c r="EF18" s="71"/>
+      <c r="EG18" s="71"/>
+      <c r="EH18" s="71"/>
+      <c r="EI18" s="71"/>
+      <c r="EJ18" s="71"/>
+      <c r="EK18" s="71"/>
+      <c r="EL18" s="71"/>
+      <c r="EM18" s="70"/>
+      <c r="EN18" s="70"/>
+      <c r="EO18" s="70"/>
+      <c r="EP18" s="70"/>
+      <c r="EQ18" s="70"/>
+      <c r="ER18" s="70"/>
+      <c r="ES18" s="70"/>
+      <c r="ET18" s="70"/>
+      <c r="EU18" s="70"/>
+      <c r="EV18" s="70"/>
+      <c r="EW18" s="70"/>
+      <c r="EX18" s="70"/>
+      <c r="EY18" s="70"/>
+      <c r="EZ18" s="70"/>
+      <c r="FA18" s="70"/>
+      <c r="FB18" s="78"/>
     </row>
     <row r="19" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B19" s="68"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="25" t="s">
         <v>212</v>
       </c>
@@ -9257,7 +9302,7 @@
       <c r="A20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B20" s="68"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="25" t="s">
         <v>322</v>
       </c>
@@ -9625,7 +9670,7 @@
       <c r="A21" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="68"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="25" t="s">
         <v>275</v>
       </c>
@@ -9941,7 +9986,7 @@
       <c r="A22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="68"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="25" t="s">
         <v>338</v>
       </c>
@@ -10235,331 +10280,331 @@
       <c r="FA22" s="26"/>
       <c r="FB22" s="28"/>
     </row>
-    <row r="23" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="b">
+    <row r="23" spans="1:158" s="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="80"/>
+      <c r="C23" s="69" t="s">
         <v>280</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="71" t="s">
         <v>278</v>
       </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35" t="s">
+      <c r="F23" s="71"/>
+      <c r="G23" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="73" t="s">
         <v>282</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="71">
+        <v>1</v>
+      </c>
+      <c r="K23" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="L23" s="71">
+        <v>605517846</v>
+      </c>
+      <c r="M23" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="N23" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="O23" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="P23" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q23" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="R23" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="S23" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71" t="s">
+        <v>345</v>
+      </c>
+      <c r="V23" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="W23" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="X23" s="71" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y23" s="71">
+        <v>9012633035</v>
+      </c>
+      <c r="Z23" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA23" s="71" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB23" s="71" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC23" s="71">
+        <v>110001</v>
+      </c>
+      <c r="AD23" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="AE23" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF23" s="71">
+        <v>214877600</v>
+      </c>
+      <c r="AG23" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH23" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI23" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ23" s="71"/>
+      <c r="AK23" s="71"/>
+      <c r="AL23" s="71"/>
+      <c r="AM23" s="71"/>
+      <c r="AN23" s="71"/>
+      <c r="AO23" s="71"/>
+      <c r="AP23" s="71"/>
+      <c r="AQ23" s="71"/>
+      <c r="AR23" s="71">
+        <v>9012633035</v>
+      </c>
+      <c r="AS23" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT23" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU23" s="71">
+        <v>9012633035</v>
+      </c>
+      <c r="AV23" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW23" s="71" t="s">
+        <v>277</v>
+      </c>
+      <c r="AX23" s="71" t="s">
+        <v>332</v>
+      </c>
+      <c r="AY23" s="76">
+        <v>110001</v>
+      </c>
+      <c r="AZ23" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="BA23" s="71" t="s">
+        <v>283</v>
+      </c>
+      <c r="BB23" s="73"/>
+      <c r="BC23" s="73"/>
+      <c r="BD23" s="73"/>
+      <c r="BE23" s="71"/>
+      <c r="BF23" s="71"/>
+      <c r="BG23" s="71"/>
+      <c r="BH23" s="71"/>
+      <c r="BI23" s="71"/>
+      <c r="BJ23" s="71"/>
+      <c r="BK23" s="71"/>
+      <c r="BL23" s="71"/>
+      <c r="BM23" s="71"/>
+      <c r="BN23" s="71"/>
+      <c r="BO23" s="71"/>
+      <c r="BP23" s="71"/>
+      <c r="BQ23" s="71"/>
+      <c r="BR23" s="71"/>
+      <c r="BS23" s="71"/>
+      <c r="BT23" s="71"/>
+      <c r="BU23" s="71"/>
+      <c r="BV23" s="71"/>
+      <c r="BW23" s="71"/>
+      <c r="BX23" s="71"/>
+      <c r="BY23" s="71"/>
+      <c r="BZ23" s="70"/>
+      <c r="CA23" s="70"/>
+      <c r="CB23" s="70"/>
+      <c r="CC23" s="70"/>
+      <c r="CD23" s="70"/>
+      <c r="CE23" s="70"/>
+      <c r="CF23" s="70"/>
+      <c r="CG23" s="70"/>
+      <c r="CH23" s="71"/>
+      <c r="CI23" s="71"/>
+      <c r="CJ23" s="77" t="s">
+        <v>248</v>
+      </c>
+      <c r="CK23" s="77">
+        <v>214877600</v>
+      </c>
+      <c r="CL23" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="CM23" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="CN23" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="CO23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CP23" s="70">
+        <v>100</v>
+      </c>
+      <c r="CQ23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CR23" s="70">
+        <v>50</v>
+      </c>
+      <c r="CS23" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="CT23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CU23" s="70">
+        <v>100</v>
+      </c>
+      <c r="CV23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="CW23" s="70">
         <v>25</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="CX23" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="CY23" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="CZ23" s="70">
+        <v>123456789</v>
+      </c>
+      <c r="DA23" s="70"/>
+      <c r="DB23" s="70"/>
+      <c r="DC23" s="70">
+        <v>1</v>
+      </c>
+      <c r="DD23" s="70" t="s">
+        <v>156</v>
+      </c>
+      <c r="DE23" s="70" t="s">
+        <v>203</v>
+      </c>
+      <c r="DF23" s="70"/>
+      <c r="DG23" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="L23" s="35">
-        <v>605517846</v>
-      </c>
-      <c r="M23" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="N23" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="O23" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="P23" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q23" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="R23" s="38" t="s">
-        <v>344</v>
-      </c>
-      <c r="S23" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35" t="s">
-        <v>345</v>
-      </c>
-      <c r="V23" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="W23" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="X23" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="Y23" s="35">
-        <v>9012633035</v>
-      </c>
-      <c r="Z23" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="AA23" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="AB23" s="35" t="s">
-        <v>332</v>
-      </c>
-      <c r="AC23" s="35">
-        <v>110001</v>
-      </c>
-      <c r="AD23" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE23" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF23" s="35">
-        <v>214877600</v>
-      </c>
-      <c r="AG23" s="26" t="s">
+      <c r="DH23" s="71">
+        <v>1</v>
+      </c>
+      <c r="DI23" s="70">
+        <v>1</v>
+      </c>
+      <c r="DJ23" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="DK23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DL23" s="70">
+        <v>100</v>
+      </c>
+      <c r="DM23" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="DN23" s="70">
+        <v>100</v>
+      </c>
+      <c r="DO23" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="DP23" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="DQ23" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="DR23" s="70">
+        <v>1</v>
+      </c>
+      <c r="DS23" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="DT23" s="71">
+        <v>100</v>
+      </c>
+      <c r="DU23" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="DV23" s="71">
+        <v>1</v>
+      </c>
+      <c r="DW23" s="71"/>
+      <c r="DX23" s="71"/>
+      <c r="DY23" s="71"/>
+      <c r="DZ23" s="71"/>
+      <c r="EA23" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="EB23" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="AH23" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="AI23" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ23" s="35"/>
-      <c r="AK23" s="35"/>
-      <c r="AL23" s="35"/>
-      <c r="AM23" s="35"/>
-      <c r="AN23" s="35"/>
-      <c r="AO23" s="35"/>
-      <c r="AP23" s="35"/>
-      <c r="AQ23" s="35"/>
-      <c r="AR23" s="35">
-        <v>9012633035</v>
-      </c>
-      <c r="AS23" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="AT23" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="AU23" s="35">
-        <v>9012633035</v>
-      </c>
-      <c r="AV23" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="AW23" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="AX23" s="35" t="s">
-        <v>332</v>
-      </c>
-      <c r="AY23" s="18">
-        <v>110001</v>
-      </c>
-      <c r="AZ23" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="BA23" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="BB23" s="17"/>
-      <c r="BC23" s="17"/>
-      <c r="BD23" s="17"/>
-      <c r="BE23" s="35"/>
-      <c r="BF23" s="35"/>
-      <c r="BG23" s="35"/>
-      <c r="BH23" s="35"/>
-      <c r="BI23" s="35"/>
-      <c r="BJ23" s="35"/>
-      <c r="BK23" s="35"/>
-      <c r="BL23" s="35"/>
-      <c r="BM23" s="35"/>
-      <c r="BN23" s="35"/>
-      <c r="BO23" s="35"/>
-      <c r="BP23" s="35"/>
-      <c r="BQ23" s="35"/>
-      <c r="BR23" s="35"/>
-      <c r="BS23" s="35"/>
-      <c r="BT23" s="35"/>
-      <c r="BU23" s="35"/>
-      <c r="BV23" s="35"/>
-      <c r="BW23" s="35"/>
-      <c r="BX23" s="35"/>
-      <c r="BY23" s="35"/>
-      <c r="BZ23" s="26"/>
-      <c r="CA23" s="26"/>
-      <c r="CB23" s="26"/>
-      <c r="CC23" s="26"/>
-      <c r="CD23" s="26"/>
-      <c r="CE23" s="26"/>
-      <c r="CF23" s="26"/>
-      <c r="CG23" s="26"/>
-      <c r="CH23" s="35"/>
-      <c r="CI23" s="35"/>
-      <c r="CJ23" s="54" t="s">
-        <v>248</v>
-      </c>
-      <c r="CK23" s="54">
-        <v>214877600</v>
-      </c>
-      <c r="CL23" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="CM23" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="CN23" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="CO23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="CP23" s="26">
-        <v>100</v>
-      </c>
-      <c r="CQ23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="CR23" s="26">
-        <v>50</v>
-      </c>
-      <c r="CS23" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="CT23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="CU23" s="26">
-        <v>100</v>
-      </c>
-      <c r="CV23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="CW23" s="26">
-        <v>25</v>
-      </c>
-      <c r="CX23" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="CY23" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="CZ23" s="26">
-        <v>123456789</v>
-      </c>
-      <c r="DA23" s="26"/>
-      <c r="DB23" s="26"/>
-      <c r="DC23" s="26">
-        <v>1</v>
-      </c>
-      <c r="DD23" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="DE23" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="DF23" s="26"/>
-      <c r="DG23" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="DH23" s="35">
-        <v>25</v>
-      </c>
-      <c r="DI23" s="26">
-        <v>1</v>
-      </c>
-      <c r="DJ23" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="DK23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="DL23" s="26">
-        <v>100</v>
-      </c>
-      <c r="DM23" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="DN23" s="26">
-        <v>100</v>
-      </c>
-      <c r="DO23" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="DP23" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="DQ23" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="DR23" s="26">
-        <v>1</v>
-      </c>
-      <c r="DS23" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="DT23" s="35">
-        <v>100</v>
-      </c>
-      <c r="DU23" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="DV23" s="35">
-        <v>25</v>
-      </c>
-      <c r="DW23" s="35"/>
-      <c r="DX23" s="35"/>
-      <c r="DY23" s="35"/>
-      <c r="DZ23" s="35"/>
-      <c r="EA23" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="EB23" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="EC23" s="35"/>
-      <c r="ED23" s="35"/>
-      <c r="EE23" s="35"/>
-      <c r="EF23" s="35"/>
-      <c r="EG23" s="35"/>
-      <c r="EH23" s="35"/>
-      <c r="EI23" s="35"/>
-      <c r="EJ23" s="35"/>
-      <c r="EK23" s="26"/>
-      <c r="EL23" s="26"/>
-      <c r="EM23" s="26"/>
-      <c r="EN23" s="26"/>
-      <c r="EO23" s="26"/>
-      <c r="EP23" s="26"/>
-      <c r="EQ23" s="26"/>
-      <c r="ER23" s="26"/>
-      <c r="ES23" s="26"/>
-      <c r="ET23" s="26"/>
-      <c r="EU23" s="26"/>
-      <c r="EV23" s="26"/>
-      <c r="EW23" s="26"/>
-      <c r="EX23" s="26"/>
-      <c r="EY23" s="26"/>
-      <c r="EZ23" s="26"/>
-      <c r="FA23" s="26"/>
-      <c r="FB23" s="28"/>
+      <c r="EC23" s="71"/>
+      <c r="ED23" s="71"/>
+      <c r="EE23" s="71"/>
+      <c r="EF23" s="71"/>
+      <c r="EG23" s="71"/>
+      <c r="EH23" s="71"/>
+      <c r="EI23" s="71"/>
+      <c r="EJ23" s="71"/>
+      <c r="EK23" s="70"/>
+      <c r="EL23" s="70"/>
+      <c r="EM23" s="70"/>
+      <c r="EN23" s="70"/>
+      <c r="EO23" s="70"/>
+      <c r="EP23" s="70"/>
+      <c r="EQ23" s="70"/>
+      <c r="ER23" s="70"/>
+      <c r="ES23" s="70"/>
+      <c r="ET23" s="70"/>
+      <c r="EU23" s="70"/>
+      <c r="EV23" s="70"/>
+      <c r="EW23" s="70"/>
+      <c r="EX23" s="70"/>
+      <c r="EY23" s="70"/>
+      <c r="EZ23" s="70"/>
+      <c r="FA23" s="70"/>
+      <c r="FB23" s="78"/>
     </row>
     <row r="24" spans="1:158" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="68"/>
+      <c r="B24" s="80"/>
       <c r="C24" s="25" t="s">
         <v>341</v>
       </c>
@@ -10913,7 +10958,7 @@
       <c r="A25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="68"/>
+      <c r="B25" s="80"/>
       <c r="C25" s="25" t="s">
         <v>346</v>
       </c>
@@ -11289,7 +11334,7 @@
       <c r="A26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="68"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="25" t="s">
         <v>327</v>
       </c>
@@ -11609,7 +11654,7 @@
       <c r="A27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="68"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="25" t="s">
         <v>325</v>
       </c>
@@ -11929,7 +11974,7 @@
       <c r="A28" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="68"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="25" t="s">
         <v>220</v>
       </c>
@@ -12269,7 +12314,7 @@
       <c r="A29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="68"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="25" t="s">
         <v>295</v>
       </c>
@@ -12609,7 +12654,7 @@
       <c r="A30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="68"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="25" t="s">
         <v>253</v>
       </c>
@@ -12959,7 +13004,7 @@
       <c r="A31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="68"/>
+      <c r="B31" s="80"/>
       <c r="C31" s="25" t="s">
         <v>235</v>
       </c>
@@ -13309,7 +13354,7 @@
       <c r="A32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="68"/>
+      <c r="B32" s="80"/>
       <c r="C32" s="25" t="s">
         <v>302</v>
       </c>
@@ -13430,8 +13475,8 @@
         <v>329</v>
       </c>
       <c r="AX32" s="35"/>
-      <c r="AY32" s="18">
-        <v>44030</v>
+      <c r="AY32" s="67" t="s">
+        <v>355</v>
       </c>
       <c r="AZ32" s="35" t="s">
         <v>168</v>
@@ -13633,7 +13678,7 @@
       <c r="A33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="68"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="25" t="s">
         <v>324</v>
       </c>
@@ -13949,7 +13994,7 @@
       <c r="A34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="68"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="25" t="s">
         <v>343</v>
       </c>
@@ -14265,7 +14310,7 @@
       <c r="A35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="68"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="25" t="s">
         <v>326</v>
       </c>
@@ -14587,7 +14632,7 @@
       <c r="A36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="68"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="25" t="s">
         <v>309</v>
       </c>
@@ -14909,7 +14954,7 @@
       <c r="A37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="68"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="25" t="s">
         <v>337</v>
       </c>
@@ -15030,8 +15075,8 @@
         <v>329</v>
       </c>
       <c r="AX37" s="35"/>
-      <c r="AY37" s="18">
-        <v>44030</v>
+      <c r="AY37" s="67" t="s">
+        <v>355</v>
       </c>
       <c r="AZ37" s="35" t="s">
         <v>168</v>
@@ -15225,7 +15270,7 @@
       <c r="A38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="68"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="25" t="s">
         <v>312</v>
       </c>
@@ -15541,7 +15586,7 @@
       <c r="A39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="68"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="25" t="s">
         <v>316</v>
       </c>
@@ -15889,7 +15934,7 @@
       <c r="A40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="68"/>
+      <c r="B40" s="80"/>
       <c r="C40" s="25" t="s">
         <v>173</v>
       </c>
@@ -16239,7 +16284,7 @@
       <c r="A41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B41" s="68"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="25" t="s">
         <v>319</v>
       </c>
@@ -16551,7 +16596,7 @@
       <c r="A42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B42" s="69"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="30" t="s">
         <v>339</v>
       </c>
@@ -16869,7 +16914,7 @@
       <c r="A43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="82" t="s">
         <v>353</v>
       </c>
       <c r="C43" s="43" t="s">
@@ -17183,7 +17228,7 @@
       <c r="A44" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="71"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="43" t="s">
         <v>323</v>
       </c>
@@ -17503,7 +17548,7 @@
       <c r="A45" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="71"/>
+      <c r="B45" s="83"/>
       <c r="C45" s="43" t="s">
         <v>340</v>
       </c>
@@ -17869,7 +17914,7 @@
       <c r="A46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="83"/>
       <c r="C46" s="43" t="s">
         <v>328</v>
       </c>
@@ -18191,7 +18236,7 @@
       <c r="A47" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="72"/>
+      <c r="B47" s="84"/>
       <c r="C47" s="43" t="s">
         <v>314</v>
       </c>

</xml_diff>

<commit_message>
TP#20444: More changes to get tests working for FedEx cert.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK International.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="356">
   <si>
     <t>Description</t>
   </si>
@@ -1216,7 +1216,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1256,6 +1256,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1907,7 +1919,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2158,6 +2170,72 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="17" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="358" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="383">
@@ -2860,8 +2938,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:FB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DW1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EJ1" sqref="EJ1"/>
+    <sheetView tabSelected="1" topLeftCell="EB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="EM11" sqref="EM11:EM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5414,353 +5492,353 @@
       <c r="FA7" s="26"/>
       <c r="FB7" s="28"/>
     </row>
-    <row r="8" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="b">
+    <row r="8" spans="1:158" s="85" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="85" t="b">
         <v>0</v>
       </c>
       <c r="B8" s="80"/>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="87" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="88" t="s">
         <v>233</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35" t="s">
+      <c r="F8" s="88"/>
+      <c r="G8" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="88">
         <v>69</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="88">
         <v>605517846</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="N8" s="35" t="s">
+      <c r="N8" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="Q8" s="35" t="s">
+      <c r="Q8" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="R8" s="38" t="s">
+      <c r="R8" s="91" t="s">
         <v>344</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="S8" s="88" t="s">
         <v>202</v>
       </c>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35" t="s">
+      <c r="T8" s="88"/>
+      <c r="U8" s="88" t="s">
         <v>345</v>
       </c>
-      <c r="V8" s="35" t="s">
+      <c r="V8" s="88" t="s">
         <v>203</v>
       </c>
-      <c r="W8" s="35" t="s">
+      <c r="W8" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="X8" s="35" t="s">
+      <c r="X8" s="88" t="s">
         <v>233</v>
       </c>
-      <c r="Y8" s="35" t="s">
+      <c r="Y8" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="Z8" s="35" t="s">
+      <c r="Z8" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="AA8" s="35" t="s">
+      <c r="AA8" s="88" t="s">
         <v>331</v>
       </c>
-      <c r="AB8" s="35" t="s">
+      <c r="AB8" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="AC8" s="35">
+      <c r="AC8" s="88">
         <v>15520</v>
       </c>
-      <c r="AD8" s="35" t="s">
+      <c r="AD8" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="AE8" s="35" t="s">
+      <c r="AE8" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="AF8" s="35" t="s">
+      <c r="AF8" s="88" t="s">
         <v>205</v>
       </c>
-      <c r="AG8" s="26" t="s">
+      <c r="AG8" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="AH8" s="59" t="s">
+      <c r="AH8" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="AI8" s="35"/>
-      <c r="AJ8" s="35"/>
-      <c r="AK8" s="35"/>
-      <c r="AL8" s="35"/>
-      <c r="AM8" s="35"/>
-      <c r="AN8" s="35"/>
-      <c r="AO8" s="35"/>
-      <c r="AP8" s="35"/>
-      <c r="AQ8" s="35"/>
-      <c r="AR8" s="35"/>
-      <c r="AS8" s="35"/>
-      <c r="AT8" s="35"/>
-      <c r="AU8" s="35"/>
-      <c r="AV8" s="35"/>
-      <c r="AW8" s="35"/>
-      <c r="AX8" s="35"/>
-      <c r="AY8" s="18"/>
-      <c r="AZ8" s="35"/>
-      <c r="BA8" s="35"/>
-      <c r="BB8" s="17">
+      <c r="AI8" s="88"/>
+      <c r="AJ8" s="88"/>
+      <c r="AK8" s="88"/>
+      <c r="AL8" s="88"/>
+      <c r="AM8" s="88"/>
+      <c r="AN8" s="88"/>
+      <c r="AO8" s="88"/>
+      <c r="AP8" s="88"/>
+      <c r="AQ8" s="88"/>
+      <c r="AR8" s="88"/>
+      <c r="AS8" s="88"/>
+      <c r="AT8" s="88"/>
+      <c r="AU8" s="88"/>
+      <c r="AV8" s="88"/>
+      <c r="AW8" s="88"/>
+      <c r="AX8" s="88"/>
+      <c r="AY8" s="93"/>
+      <c r="AZ8" s="88"/>
+      <c r="BA8" s="88"/>
+      <c r="BB8" s="90">
         <v>1</v>
       </c>
-      <c r="BC8" s="17">
+      <c r="BC8" s="90">
         <v>101</v>
       </c>
-      <c r="BD8" s="17">
+      <c r="BD8" s="90">
         <v>123456789</v>
       </c>
-      <c r="BE8" s="35" t="s">
+      <c r="BE8" s="88" t="s">
         <v>195</v>
       </c>
-      <c r="BF8" s="35">
+      <c r="BF8" s="88">
         <v>222326460</v>
       </c>
-      <c r="BG8" s="35" t="s">
+      <c r="BG8" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="BH8" s="35">
+      <c r="BH8" s="88">
         <v>1234567890</v>
       </c>
-      <c r="BI8" s="35">
+      <c r="BI8" s="88">
         <v>12345</v>
       </c>
-      <c r="BJ8" s="35" t="s">
+      <c r="BJ8" s="88" t="s">
         <v>222</v>
       </c>
-      <c r="BK8" s="35" t="s">
+      <c r="BK8" s="88" t="s">
         <v>196</v>
       </c>
-      <c r="BL8" s="35" t="s">
+      <c r="BL8" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="BM8" s="35">
+      <c r="BM8" s="88">
         <v>8975898616</v>
       </c>
-      <c r="BN8" s="35">
+      <c r="BN8" s="88">
         <v>3293</v>
       </c>
-      <c r="BO8" s="35" t="s">
+      <c r="BO8" s="88" t="s">
         <v>197</v>
       </c>
-      <c r="BP8" s="35" t="s">
+      <c r="BP8" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="BQ8" s="35" t="s">
+      <c r="BQ8" s="88" t="s">
         <v>226</v>
       </c>
-      <c r="BR8" s="35" t="s">
+      <c r="BR8" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="BS8" s="35">
+      <c r="BS8" s="88">
         <v>15520</v>
       </c>
-      <c r="BT8" s="35" t="s">
+      <c r="BT8" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="BU8" s="35"/>
-      <c r="BV8" s="35"/>
-      <c r="BW8" s="35"/>
-      <c r="BX8" s="35"/>
-      <c r="BY8" s="35"/>
-      <c r="BZ8" s="35"/>
-      <c r="CA8" s="35"/>
-      <c r="CB8" s="35"/>
-      <c r="CC8" s="35"/>
-      <c r="CD8" s="35"/>
-      <c r="CE8" s="35"/>
-      <c r="CF8" s="35"/>
-      <c r="CG8" s="35"/>
-      <c r="CH8" s="35" t="s">
+      <c r="BU8" s="88"/>
+      <c r="BV8" s="88"/>
+      <c r="BW8" s="88"/>
+      <c r="BX8" s="88"/>
+      <c r="BY8" s="88"/>
+      <c r="BZ8" s="88"/>
+      <c r="CA8" s="88"/>
+      <c r="CB8" s="88"/>
+      <c r="CC8" s="88"/>
+      <c r="CD8" s="88"/>
+      <c r="CE8" s="88"/>
+      <c r="CF8" s="88"/>
+      <c r="CG8" s="88"/>
+      <c r="CH8" s="88" t="s">
         <v>192</v>
       </c>
-      <c r="CI8" s="35">
+      <c r="CI8" s="88">
         <v>12345678</v>
       </c>
-      <c r="CJ8" s="54" t="s">
+      <c r="CJ8" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="CK8" s="54" t="s">
+      <c r="CK8" s="94" t="s">
         <v>215</v>
       </c>
-      <c r="CL8" s="35" t="s">
+      <c r="CL8" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="CM8" s="59" t="s">
+      <c r="CM8" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="CN8" s="26" t="s">
+      <c r="CN8" s="87" t="s">
         <v>190</v>
       </c>
-      <c r="CO8" s="26" t="s">
+      <c r="CO8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="CP8" s="26">
+      <c r="CP8" s="87">
         <v>2000</v>
       </c>
-      <c r="CQ8" s="26" t="s">
+      <c r="CQ8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="CR8" s="26">
+      <c r="CR8" s="87">
         <v>50</v>
       </c>
-      <c r="CS8" s="26" t="s">
+      <c r="CS8" s="87" t="s">
         <v>153</v>
       </c>
-      <c r="CT8" s="26" t="s">
+      <c r="CT8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="CU8" s="26">
+      <c r="CU8" s="87">
         <v>100</v>
       </c>
-      <c r="CV8" s="26" t="s">
+      <c r="CV8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="CW8" s="26">
+      <c r="CW8" s="87">
         <v>25</v>
       </c>
-      <c r="CX8" s="26" t="s">
+      <c r="CX8" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="CY8" s="26" t="s">
+      <c r="CY8" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="CZ8" s="26">
+      <c r="CZ8" s="87">
         <v>123456789</v>
       </c>
-      <c r="DA8" s="26"/>
-      <c r="DB8" s="26"/>
-      <c r="DC8" s="26">
+      <c r="DA8" s="87"/>
+      <c r="DB8" s="87"/>
+      <c r="DC8" s="87">
         <v>1</v>
       </c>
-      <c r="DD8" s="26" t="s">
+      <c r="DD8" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="DE8" s="26" t="s">
+      <c r="DE8" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="DF8" s="26"/>
-      <c r="DG8" s="26" t="s">
+      <c r="DF8" s="87"/>
+      <c r="DG8" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="DH8" s="35">
+      <c r="DH8" s="88">
         <v>69</v>
       </c>
-      <c r="DI8" s="26">
+      <c r="DI8" s="87">
         <v>1</v>
       </c>
-      <c r="DJ8" s="26" t="s">
+      <c r="DJ8" s="87" t="s">
         <v>158</v>
       </c>
-      <c r="DK8" s="26" t="s">
+      <c r="DK8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="DL8" s="26">
+      <c r="DL8" s="87">
         <v>100</v>
       </c>
-      <c r="DM8" s="26" t="s">
+      <c r="DM8" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="DN8" s="26">
+      <c r="DN8" s="87">
         <v>2000</v>
       </c>
-      <c r="DO8" s="26" t="s">
+      <c r="DO8" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="DP8" s="35" t="s">
+      <c r="DP8" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="DQ8" s="35" t="s">
+      <c r="DQ8" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="DR8" s="26">
+      <c r="DR8" s="87">
         <v>1</v>
       </c>
-      <c r="DS8" s="35" t="s">
+      <c r="DS8" s="88" t="s">
         <v>152</v>
       </c>
-      <c r="DT8" s="35">
+      <c r="DT8" s="88">
         <v>800</v>
       </c>
-      <c r="DU8" s="35" t="s">
+      <c r="DU8" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="DV8" s="35">
+      <c r="DV8" s="88">
         <v>69</v>
       </c>
-      <c r="DW8" s="35">
+      <c r="DW8" s="88">
         <v>20</v>
       </c>
-      <c r="DX8" s="35">
+      <c r="DX8" s="88">
         <v>20</v>
       </c>
-      <c r="DY8" s="35">
+      <c r="DY8" s="88">
         <v>20</v>
       </c>
-      <c r="DZ8" s="35" t="s">
+      <c r="DZ8" s="88" t="s">
         <v>163</v>
       </c>
-      <c r="EA8" s="35" t="s">
+      <c r="EA8" s="88" t="s">
         <v>155</v>
       </c>
-      <c r="EB8" s="35" t="s">
+      <c r="EB8" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="EC8" s="35"/>
-      <c r="ED8" s="35"/>
-      <c r="EE8" s="35"/>
-      <c r="EF8" s="35"/>
-      <c r="EG8" s="35"/>
-      <c r="EH8" s="35"/>
-      <c r="EI8" s="35"/>
-      <c r="EJ8" s="35"/>
-      <c r="EK8" s="35"/>
-      <c r="EL8" s="35"/>
-      <c r="EM8" s="26"/>
-      <c r="EN8" s="26"/>
-      <c r="EO8" s="26"/>
-      <c r="EP8" s="26"/>
-      <c r="EQ8" s="26"/>
-      <c r="ER8" s="26"/>
-      <c r="ES8" s="26"/>
-      <c r="ET8" s="26"/>
-      <c r="EU8" s="26"/>
-      <c r="EV8" s="26"/>
-      <c r="EW8" s="26"/>
-      <c r="EX8" s="26"/>
-      <c r="EY8" s="26"/>
-      <c r="EZ8" s="26"/>
-      <c r="FA8" s="26"/>
-      <c r="FB8" s="28"/>
+      <c r="EC8" s="88"/>
+      <c r="ED8" s="88"/>
+      <c r="EE8" s="88"/>
+      <c r="EF8" s="88"/>
+      <c r="EG8" s="88"/>
+      <c r="EH8" s="88"/>
+      <c r="EI8" s="88"/>
+      <c r="EJ8" s="88"/>
+      <c r="EK8" s="88"/>
+      <c r="EL8" s="88"/>
+      <c r="EM8" s="87"/>
+      <c r="EN8" s="87"/>
+      <c r="EO8" s="87"/>
+      <c r="EP8" s="87"/>
+      <c r="EQ8" s="87"/>
+      <c r="ER8" s="87"/>
+      <c r="ES8" s="87"/>
+      <c r="ET8" s="87"/>
+      <c r="EU8" s="87"/>
+      <c r="EV8" s="87"/>
+      <c r="EW8" s="87"/>
+      <c r="EX8" s="87"/>
+      <c r="EY8" s="87"/>
+      <c r="EZ8" s="87"/>
+      <c r="FA8" s="87"/>
+      <c r="FB8" s="95"/>
     </row>
     <row r="9" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="b">
@@ -6414,689 +6492,685 @@
       <c r="FA10" s="26"/>
       <c r="FB10" s="28"/>
     </row>
-    <row r="11" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="b">
+    <row r="11" spans="1:158" s="96" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="96" t="b">
         <v>0</v>
       </c>
       <c r="B11" s="80"/>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="97" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="98" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35" t="s">
+      <c r="F11" s="99"/>
+      <c r="G11" s="99" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="J11" s="35">
+      <c r="J11" s="99">
         <v>30</v>
       </c>
-      <c r="K11" s="35" t="s">
+      <c r="K11" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="99">
         <v>605517846</v>
       </c>
-      <c r="M11" s="35" t="s">
+      <c r="M11" s="99" t="s">
         <v>144</v>
       </c>
-      <c r="N11" s="35" t="s">
+      <c r="N11" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="O11" s="35" t="s">
+      <c r="O11" s="99" t="s">
         <v>146</v>
       </c>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="Q11" s="35" t="s">
+      <c r="Q11" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="R11" s="38" t="s">
+      <c r="R11" s="102" t="s">
         <v>344</v>
       </c>
-      <c r="S11" s="35" t="s">
+      <c r="S11" s="99" t="s">
         <v>202</v>
       </c>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35" t="s">
+      <c r="T11" s="99"/>
+      <c r="U11" s="99" t="s">
         <v>345</v>
       </c>
-      <c r="V11" s="35" t="s">
+      <c r="V11" s="99" t="s">
         <v>203</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="W11" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="X11" s="35" t="s">
+      <c r="X11" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="Y11" s="35" t="s">
+      <c r="Y11" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="Z11" s="35" t="s">
+      <c r="Z11" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="AA11" s="35" t="s">
+      <c r="AA11" s="99" t="s">
         <v>237</v>
       </c>
-      <c r="AB11" s="35" t="s">
+      <c r="AB11" s="99" t="s">
         <v>238</v>
       </c>
-      <c r="AC11" s="35">
+      <c r="AC11" s="99">
         <v>30339</v>
       </c>
-      <c r="AD11" s="35" t="s">
+      <c r="AD11" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="AE11" s="35" t="s">
+      <c r="AE11" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="AF11" s="35" t="s">
+      <c r="AF11" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="AG11" s="26" t="s">
+      <c r="AG11" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="AH11" s="59" t="s">
+      <c r="AH11" s="103" t="s">
         <v>203</v>
       </c>
-      <c r="AI11" s="35"/>
-      <c r="AJ11" s="35"/>
-      <c r="AK11" s="35"/>
-      <c r="AL11" s="35"/>
-      <c r="AM11" s="35"/>
-      <c r="AN11" s="35"/>
-      <c r="AO11" s="35"/>
-      <c r="AP11" s="35"/>
-      <c r="AQ11" s="35"/>
-      <c r="AR11" s="35"/>
-      <c r="AS11" s="35"/>
-      <c r="AT11" s="35"/>
-      <c r="AU11" s="35"/>
-      <c r="AV11" s="35"/>
-      <c r="AW11" s="35"/>
-      <c r="AX11" s="35"/>
-      <c r="AY11" s="18"/>
-      <c r="AZ11" s="35"/>
-      <c r="BA11" s="35"/>
-      <c r="BB11" s="17"/>
-      <c r="BC11" s="17"/>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="35"/>
-      <c r="BF11" s="35"/>
-      <c r="BG11" s="35"/>
-      <c r="BH11" s="35"/>
-      <c r="BI11" s="35"/>
-      <c r="BJ11" s="35"/>
-      <c r="BK11" s="35"/>
-      <c r="BL11" s="35"/>
-      <c r="BM11" s="35"/>
-      <c r="BN11" s="35"/>
-      <c r="BO11" s="35"/>
-      <c r="BP11" s="35"/>
-      <c r="BQ11" s="35"/>
-      <c r="BR11" s="35"/>
-      <c r="BS11" s="35"/>
-      <c r="BT11" s="35"/>
-      <c r="BU11" s="35"/>
-      <c r="BV11" s="35"/>
-      <c r="BW11" s="35"/>
-      <c r="BX11" s="35"/>
-      <c r="BY11" s="35"/>
-      <c r="BZ11" s="35"/>
-      <c r="CA11" s="35"/>
-      <c r="CB11" s="35"/>
-      <c r="CC11" s="35"/>
-      <c r="CD11" s="35"/>
-      <c r="CE11" s="35"/>
-      <c r="CF11" s="35"/>
-      <c r="CG11" s="35"/>
-      <c r="CH11" s="35"/>
-      <c r="CI11" s="35"/>
-      <c r="CJ11" s="54" t="s">
+      <c r="AI11" s="99"/>
+      <c r="AJ11" s="99"/>
+      <c r="AK11" s="99"/>
+      <c r="AL11" s="99"/>
+      <c r="AM11" s="99"/>
+      <c r="AN11" s="99"/>
+      <c r="AO11" s="99"/>
+      <c r="AP11" s="99"/>
+      <c r="AQ11" s="99"/>
+      <c r="AR11" s="99"/>
+      <c r="AS11" s="99"/>
+      <c r="AT11" s="99"/>
+      <c r="AU11" s="99"/>
+      <c r="AV11" s="99"/>
+      <c r="AW11" s="99"/>
+      <c r="AX11" s="99"/>
+      <c r="AY11" s="104"/>
+      <c r="AZ11" s="99"/>
+      <c r="BA11" s="99"/>
+      <c r="BB11" s="101"/>
+      <c r="BC11" s="101"/>
+      <c r="BD11" s="101"/>
+      <c r="BE11" s="99"/>
+      <c r="BF11" s="99"/>
+      <c r="BG11" s="99"/>
+      <c r="BH11" s="99"/>
+      <c r="BI11" s="99"/>
+      <c r="BJ11" s="99"/>
+      <c r="BK11" s="99"/>
+      <c r="BL11" s="99"/>
+      <c r="BM11" s="99"/>
+      <c r="BN11" s="99"/>
+      <c r="BO11" s="99"/>
+      <c r="BP11" s="99"/>
+      <c r="BQ11" s="99"/>
+      <c r="BR11" s="99"/>
+      <c r="BS11" s="99"/>
+      <c r="BT11" s="99"/>
+      <c r="BU11" s="99"/>
+      <c r="BV11" s="99"/>
+      <c r="BW11" s="99"/>
+      <c r="BX11" s="99"/>
+      <c r="BY11" s="99"/>
+      <c r="BZ11" s="99"/>
+      <c r="CA11" s="99"/>
+      <c r="CB11" s="99"/>
+      <c r="CC11" s="99"/>
+      <c r="CD11" s="99"/>
+      <c r="CE11" s="99"/>
+      <c r="CF11" s="99"/>
+      <c r="CG11" s="99"/>
+      <c r="CH11" s="99"/>
+      <c r="CI11" s="99"/>
+      <c r="CJ11" s="105" t="s">
         <v>149</v>
       </c>
-      <c r="CK11" s="54" t="s">
+      <c r="CK11" s="105" t="s">
         <v>215</v>
       </c>
-      <c r="CL11" s="35" t="s">
+      <c r="CL11" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="CM11" s="59" t="s">
+      <c r="CM11" s="103" t="s">
         <v>203</v>
       </c>
-      <c r="CN11" s="26" t="s">
+      <c r="CN11" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="CO11" s="26" t="s">
+      <c r="CO11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CP11" s="26">
+      <c r="CP11" s="98">
         <v>55</v>
       </c>
-      <c r="CQ11" s="26" t="s">
+      <c r="CQ11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CR11" s="26">
+      <c r="CR11" s="98">
         <v>50</v>
       </c>
-      <c r="CS11" s="26" t="s">
+      <c r="CS11" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="CT11" s="26" t="s">
+      <c r="CT11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CU11" s="26">
+      <c r="CU11" s="98">
         <v>100</v>
       </c>
-      <c r="CV11" s="26" t="s">
+      <c r="CV11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CW11" s="26">
+      <c r="CW11" s="98">
         <v>25</v>
       </c>
-      <c r="CX11" s="26" t="s">
+      <c r="CX11" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="CY11" s="26" t="s">
+      <c r="CY11" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="CZ11" s="26">
+      <c r="CZ11" s="98">
         <v>123456789</v>
       </c>
-      <c r="DA11" s="26"/>
-      <c r="DB11" s="26"/>
-      <c r="DC11" s="26">
+      <c r="DA11" s="98"/>
+      <c r="DB11" s="98"/>
+      <c r="DC11" s="98">
         <v>1</v>
       </c>
-      <c r="DD11" s="26" t="s">
+      <c r="DD11" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="DE11" s="26" t="s">
+      <c r="DE11" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="DF11" s="26"/>
-      <c r="DG11" s="26" t="s">
+      <c r="DF11" s="98"/>
+      <c r="DG11" s="98" t="s">
         <v>162</v>
       </c>
-      <c r="DH11" s="35">
+      <c r="DH11" s="99">
         <v>30</v>
       </c>
-      <c r="DI11" s="26">
+      <c r="DI11" s="98">
         <v>1</v>
       </c>
-      <c r="DJ11" s="26" t="s">
+      <c r="DJ11" s="98" t="s">
         <v>158</v>
       </c>
-      <c r="DK11" s="26" t="s">
+      <c r="DK11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="DL11" s="26">
+      <c r="DL11" s="98">
         <v>100</v>
       </c>
-      <c r="DM11" s="26" t="s">
+      <c r="DM11" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="DN11" s="26">
+      <c r="DN11" s="98">
         <v>55</v>
       </c>
-      <c r="DO11" s="26" t="s">
+      <c r="DO11" s="98" t="s">
         <v>159</v>
       </c>
-      <c r="DP11" s="35" t="s">
+      <c r="DP11" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="DQ11" s="35" t="s">
+      <c r="DQ11" s="99" t="s">
         <v>223</v>
       </c>
-      <c r="DR11" s="26">
+      <c r="DR11" s="98">
         <v>1</v>
       </c>
-      <c r="DS11" s="35" t="s">
+      <c r="DS11" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="DT11" s="35">
+      <c r="DT11" s="99">
         <v>55</v>
       </c>
-      <c r="DU11" s="35" t="s">
+      <c r="DU11" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="DV11" s="35">
+      <c r="DV11" s="99">
         <v>30</v>
       </c>
-      <c r="DW11" s="35">
+      <c r="DW11" s="99">
         <v>20</v>
       </c>
-      <c r="DX11" s="35">
+      <c r="DX11" s="99">
         <v>20</v>
       </c>
-      <c r="DY11" s="35">
+      <c r="DY11" s="99">
         <v>20</v>
       </c>
-      <c r="DZ11" s="35" t="s">
+      <c r="DZ11" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="EA11" s="35" t="s">
+      <c r="EA11" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="EB11" s="35" t="s">
+      <c r="EB11" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="EC11" s="35" t="s">
+      <c r="EC11" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="ED11" s="35"/>
-      <c r="EE11" s="35"/>
-      <c r="EF11" s="35"/>
-      <c r="EG11" s="35"/>
-      <c r="EH11" s="35"/>
-      <c r="EI11" s="35"/>
-      <c r="EJ11" s="35"/>
-      <c r="EK11" s="35" t="s">
+      <c r="ED11" s="99"/>
+      <c r="EE11" s="99"/>
+      <c r="EF11" s="99"/>
+      <c r="EG11" s="99"/>
+      <c r="EH11" s="99"/>
+      <c r="EI11" s="99"/>
+      <c r="EJ11" s="99"/>
+      <c r="EK11" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="EL11" s="35"/>
-      <c r="EM11" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="EN11" s="26" t="s">
+      <c r="EL11" s="99"/>
+      <c r="EM11" s="98"/>
+      <c r="EN11" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="EO11" s="26">
+      <c r="EO11" s="98">
         <v>1</v>
       </c>
-      <c r="EP11" s="26">
+      <c r="EP11" s="98">
         <v>1090</v>
       </c>
-      <c r="EQ11" s="26">
+      <c r="EQ11" s="98">
         <v>1</v>
       </c>
-      <c r="ER11" s="26" t="s">
+      <c r="ER11" s="98" t="s">
         <v>178</v>
       </c>
-      <c r="ES11" s="26">
+      <c r="ES11" s="98">
         <v>0</v>
       </c>
-      <c r="ET11" s="26" t="s">
+      <c r="ET11" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="EU11" s="26" t="s">
+      <c r="EU11" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="EV11" s="26">
+      <c r="EV11" s="98">
         <v>3</v>
       </c>
-      <c r="EW11" s="26">
+      <c r="EW11" s="98">
         <v>1</v>
       </c>
-      <c r="EX11" s="26" t="s">
+      <c r="EX11" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="EY11" s="26" t="s">
+      <c r="EY11" s="98" t="s">
         <v>243</v>
       </c>
-      <c r="EZ11" s="26" t="s">
+      <c r="EZ11" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="FA11" s="26" t="s">
+      <c r="FA11" s="98" t="s">
         <v>245</v>
       </c>
-      <c r="FB11" s="28">
+      <c r="FB11" s="106">
         <v>9015551234</v>
       </c>
     </row>
-    <row r="12" spans="1:158" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="b">
+    <row r="12" spans="1:158" s="96" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="96" t="b">
         <v>0</v>
       </c>
       <c r="B12" s="80"/>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="97" t="s">
         <v>246</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="98" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="99"/>
+      <c r="G12" s="99" t="s">
         <v>164</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="J12" s="35">
+      <c r="J12" s="99">
         <v>50</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="L12" s="35">
+      <c r="L12" s="99">
         <v>605517846</v>
       </c>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="99" t="s">
         <v>144</v>
       </c>
-      <c r="N12" s="35" t="s">
+      <c r="N12" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="O12" s="35" t="s">
+      <c r="O12" s="99" t="s">
         <v>146</v>
       </c>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="Q12" s="35" t="s">
+      <c r="Q12" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="R12" s="38" t="s">
+      <c r="R12" s="102" t="s">
         <v>344</v>
       </c>
-      <c r="S12" s="35" t="s">
+      <c r="S12" s="99" t="s">
         <v>202</v>
       </c>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35" t="s">
+      <c r="T12" s="99"/>
+      <c r="U12" s="99" t="s">
         <v>345</v>
       </c>
-      <c r="V12" s="35" t="s">
+      <c r="V12" s="99" t="s">
         <v>203</v>
       </c>
-      <c r="W12" s="35" t="s">
+      <c r="W12" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="X12" s="35" t="s">
+      <c r="X12" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="Y12" s="35" t="s">
+      <c r="Y12" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="Z12" s="35" t="s">
+      <c r="Z12" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="AA12" s="35" t="s">
+      <c r="AA12" s="99" t="s">
         <v>334</v>
       </c>
-      <c r="AB12" s="35" t="s">
+      <c r="AB12" s="99" t="s">
         <v>172</v>
       </c>
-      <c r="AC12" s="35">
+      <c r="AC12" s="99">
         <v>38117</v>
       </c>
-      <c r="AD12" s="35" t="s">
+      <c r="AD12" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="AE12" s="35" t="s">
+      <c r="AE12" s="99" t="s">
         <v>248</v>
       </c>
-      <c r="AF12" s="35">
+      <c r="AF12" s="99">
         <v>150067600</v>
       </c>
-      <c r="AG12" s="26" t="s">
+      <c r="AG12" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="AH12" s="59" t="s">
+      <c r="AH12" s="103" t="s">
         <v>157</v>
       </c>
-      <c r="AI12" s="35"/>
-      <c r="AJ12" s="35"/>
-      <c r="AK12" s="35"/>
-      <c r="AL12" s="35"/>
-      <c r="AM12" s="35"/>
-      <c r="AN12" s="35"/>
-      <c r="AO12" s="35"/>
-      <c r="AP12" s="35"/>
-      <c r="AQ12" s="35"/>
-      <c r="AR12" s="35"/>
-      <c r="AS12" s="35"/>
-      <c r="AT12" s="35"/>
-      <c r="AU12" s="35"/>
-      <c r="AV12" s="35"/>
-      <c r="AW12" s="35"/>
-      <c r="AX12" s="35"/>
-      <c r="AY12" s="18"/>
-      <c r="AZ12" s="35"/>
-      <c r="BA12" s="35"/>
-      <c r="BB12" s="17"/>
-      <c r="BC12" s="17"/>
-      <c r="BD12" s="17"/>
-      <c r="BE12" s="35"/>
-      <c r="BF12" s="35"/>
-      <c r="BG12" s="35"/>
-      <c r="BH12" s="35"/>
-      <c r="BI12" s="35"/>
-      <c r="BJ12" s="35"/>
-      <c r="BK12" s="35"/>
-      <c r="BL12" s="35"/>
-      <c r="BM12" s="35"/>
-      <c r="BN12" s="35"/>
-      <c r="BO12" s="35"/>
-      <c r="BP12" s="35"/>
-      <c r="BQ12" s="35"/>
-      <c r="BR12" s="35"/>
-      <c r="BS12" s="35"/>
-      <c r="BT12" s="35"/>
-      <c r="BU12" s="35"/>
-      <c r="BV12" s="35"/>
-      <c r="BW12" s="35"/>
-      <c r="BX12" s="35"/>
-      <c r="BY12" s="35"/>
-      <c r="BZ12" s="35"/>
-      <c r="CA12" s="35"/>
-      <c r="CB12" s="35"/>
-      <c r="CC12" s="35"/>
-      <c r="CD12" s="35"/>
-      <c r="CE12" s="35"/>
-      <c r="CF12" s="35"/>
-      <c r="CG12" s="35"/>
-      <c r="CH12" s="35"/>
-      <c r="CI12" s="35"/>
-      <c r="CJ12" s="54" t="s">
+      <c r="AI12" s="99"/>
+      <c r="AJ12" s="99"/>
+      <c r="AK12" s="99"/>
+      <c r="AL12" s="99"/>
+      <c r="AM12" s="99"/>
+      <c r="AN12" s="99"/>
+      <c r="AO12" s="99"/>
+      <c r="AP12" s="99"/>
+      <c r="AQ12" s="99"/>
+      <c r="AR12" s="99"/>
+      <c r="AS12" s="99"/>
+      <c r="AT12" s="99"/>
+      <c r="AU12" s="99"/>
+      <c r="AV12" s="99"/>
+      <c r="AW12" s="99"/>
+      <c r="AX12" s="99"/>
+      <c r="AY12" s="104"/>
+      <c r="AZ12" s="99"/>
+      <c r="BA12" s="99"/>
+      <c r="BB12" s="101"/>
+      <c r="BC12" s="101"/>
+      <c r="BD12" s="101"/>
+      <c r="BE12" s="99"/>
+      <c r="BF12" s="99"/>
+      <c r="BG12" s="99"/>
+      <c r="BH12" s="99"/>
+      <c r="BI12" s="99"/>
+      <c r="BJ12" s="99"/>
+      <c r="BK12" s="99"/>
+      <c r="BL12" s="99"/>
+      <c r="BM12" s="99"/>
+      <c r="BN12" s="99"/>
+      <c r="BO12" s="99"/>
+      <c r="BP12" s="99"/>
+      <c r="BQ12" s="99"/>
+      <c r="BR12" s="99"/>
+      <c r="BS12" s="99"/>
+      <c r="BT12" s="99"/>
+      <c r="BU12" s="99"/>
+      <c r="BV12" s="99"/>
+      <c r="BW12" s="99"/>
+      <c r="BX12" s="99"/>
+      <c r="BY12" s="99"/>
+      <c r="BZ12" s="99"/>
+      <c r="CA12" s="99"/>
+      <c r="CB12" s="99"/>
+      <c r="CC12" s="99"/>
+      <c r="CD12" s="99"/>
+      <c r="CE12" s="99"/>
+      <c r="CF12" s="99"/>
+      <c r="CG12" s="99"/>
+      <c r="CH12" s="99"/>
+      <c r="CI12" s="99"/>
+      <c r="CJ12" s="105" t="s">
         <v>248</v>
       </c>
-      <c r="CK12" s="54">
+      <c r="CK12" s="105">
         <v>214877600</v>
       </c>
-      <c r="CL12" s="35" t="s">
+      <c r="CL12" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="CM12" s="59" t="s">
+      <c r="CM12" s="103" t="s">
         <v>157</v>
       </c>
-      <c r="CN12" s="26" t="s">
+      <c r="CN12" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="CO12" s="26" t="s">
+      <c r="CO12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CP12" s="26">
+      <c r="CP12" s="98">
         <v>200</v>
       </c>
-      <c r="CQ12" s="26" t="s">
+      <c r="CQ12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CR12" s="26">
+      <c r="CR12" s="98">
         <v>50</v>
       </c>
-      <c r="CS12" s="26" t="s">
+      <c r="CS12" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="CT12" s="26" t="s">
+      <c r="CT12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CU12" s="26">
+      <c r="CU12" s="98">
         <v>100</v>
       </c>
-      <c r="CV12" s="26" t="s">
+      <c r="CV12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="CW12" s="26">
+      <c r="CW12" s="98">
         <v>25</v>
       </c>
-      <c r="CX12" s="26" t="s">
+      <c r="CX12" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="CY12" s="26" t="s">
+      <c r="CY12" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="CZ12" s="26">
+      <c r="CZ12" s="98">
         <v>123456789</v>
       </c>
-      <c r="DA12" s="26"/>
-      <c r="DB12" s="26"/>
-      <c r="DC12" s="26">
+      <c r="DA12" s="98"/>
+      <c r="DB12" s="98"/>
+      <c r="DC12" s="98">
         <v>1</v>
       </c>
-      <c r="DD12" s="26" t="s">
+      <c r="DD12" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="DE12" s="26" t="s">
+      <c r="DE12" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="DF12" s="26"/>
-      <c r="DG12" s="26" t="s">
+      <c r="DF12" s="98"/>
+      <c r="DG12" s="98" t="s">
         <v>162</v>
       </c>
-      <c r="DH12" s="35">
+      <c r="DH12" s="99">
         <v>50</v>
       </c>
-      <c r="DI12" s="26">
+      <c r="DI12" s="98">
         <v>1</v>
       </c>
-      <c r="DJ12" s="26" t="s">
+      <c r="DJ12" s="98" t="s">
         <v>158</v>
       </c>
-      <c r="DK12" s="26" t="s">
+      <c r="DK12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="DL12" s="26">
+      <c r="DL12" s="98">
         <v>100</v>
       </c>
-      <c r="DM12" s="26" t="s">
+      <c r="DM12" s="98" t="s">
         <v>152</v>
       </c>
-      <c r="DN12" s="26">
+      <c r="DN12" s="98">
         <v>200</v>
       </c>
-      <c r="DO12" s="26" t="s">
+      <c r="DO12" s="98" t="s">
         <v>159</v>
       </c>
-      <c r="DP12" s="35" t="s">
+      <c r="DP12" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="DQ12" s="35" t="s">
+      <c r="DQ12" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="DR12" s="26">
+      <c r="DR12" s="98">
         <v>1</v>
       </c>
-      <c r="DS12" s="35" t="s">
+      <c r="DS12" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="DT12" s="35">
+      <c r="DT12" s="99">
         <v>100</v>
       </c>
-      <c r="DU12" s="35" t="s">
+      <c r="DU12" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="DV12" s="35">
+      <c r="DV12" s="99">
         <v>50</v>
       </c>
-      <c r="DW12" s="35">
+      <c r="DW12" s="99">
         <v>20</v>
       </c>
-      <c r="DX12" s="35">
+      <c r="DX12" s="99">
         <v>15</v>
       </c>
-      <c r="DY12" s="35">
+      <c r="DY12" s="99">
         <v>20</v>
       </c>
-      <c r="DZ12" s="35" t="s">
+      <c r="DZ12" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="EA12" s="35" t="s">
+      <c r="EA12" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="EB12" s="35" t="s">
+      <c r="EB12" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="EC12" s="35" t="s">
+      <c r="EC12" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="ED12" s="35"/>
-      <c r="EE12" s="35"/>
-      <c r="EF12" s="35"/>
-      <c r="EG12" s="35"/>
-      <c r="EH12" s="35"/>
-      <c r="EI12" s="35"/>
-      <c r="EJ12" s="35"/>
-      <c r="EK12" s="35" t="s">
+      <c r="ED12" s="99"/>
+      <c r="EE12" s="99"/>
+      <c r="EF12" s="99"/>
+      <c r="EG12" s="99"/>
+      <c r="EH12" s="99"/>
+      <c r="EI12" s="99"/>
+      <c r="EJ12" s="99"/>
+      <c r="EK12" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="EL12" s="35">
+      <c r="EL12" s="99">
         <v>1</v>
       </c>
-      <c r="EM12" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="EN12" s="26" t="s">
+      <c r="EM12" s="98"/>
+      <c r="EN12" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="EO12" s="26">
+      <c r="EO12" s="98">
         <v>1</v>
       </c>
-      <c r="EP12" s="26">
+      <c r="EP12" s="98">
         <v>1888</v>
       </c>
-      <c r="EQ12" s="26">
+      <c r="EQ12" s="98">
         <v>1</v>
       </c>
-      <c r="ER12" s="26" t="s">
+      <c r="ER12" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="ES12" s="26">
+      <c r="ES12" s="98">
         <v>1</v>
       </c>
-      <c r="ET12" s="26">
+      <c r="ET12" s="98">
         <v>680</v>
       </c>
-      <c r="EU12" s="26" t="s">
+      <c r="EU12" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="EV12" s="26">
+      <c r="EV12" s="98">
         <v>6.1</v>
       </c>
-      <c r="EW12" s="26">
+      <c r="EW12" s="98">
         <v>1</v>
       </c>
-      <c r="EX12" s="26" t="s">
+      <c r="EX12" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="EY12" s="26" t="s">
+      <c r="EY12" s="98" t="s">
         <v>243</v>
       </c>
-      <c r="EZ12" s="26" t="s">
+      <c r="EZ12" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="FA12" s="26" t="s">
+      <c r="FA12" s="98" t="s">
         <v>245</v>
       </c>
-      <c r="FB12" s="28">
+      <c r="FB12" s="106">
         <v>9015551234</v>
       </c>
     </row>

</xml_diff>